<commit_message>
updated Unity, readme, music list
</commit_message>
<xml_diff>
--- a/MusicList.xlsx
+++ b/MusicList.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
   <si>
     <t>Disco</t>
   </si>
@@ -281,13 +281,25 @@
   </si>
   <si>
     <t>Chill out / Chill House</t>
+  </si>
+  <si>
+    <t>Genres</t>
+  </si>
+  <si>
+    <t>Blues</t>
+  </si>
+  <si>
+    <t>Video Game / Chiptune</t>
+  </si>
+  <si>
+    <t>Pop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,8 +315,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,8 +335,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -326,11 +350,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -347,11 +382,93 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -436,28 +553,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P53" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P53" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:P53"/>
   <sortState ref="A2:P55">
     <sortCondition ref="C1:C55"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="Music Genre" dataDxfId="15"/>
-    <tableColumn id="16" name="Column1" dataDxfId="14"/>
-    <tableColumn id="15" name="Using" dataDxfId="13"/>
-    <tableColumn id="2" name="Column13" dataDxfId="12"/>
-    <tableColumn id="3" name="Column2" dataDxfId="11"/>
-    <tableColumn id="4" name="Column3" dataDxfId="10"/>
-    <tableColumn id="5" name="Column4" dataDxfId="9"/>
-    <tableColumn id="6" name="Column5" dataDxfId="8"/>
-    <tableColumn id="8" name="Column52" dataDxfId="7"/>
-    <tableColumn id="7" name="Column6" dataDxfId="6"/>
-    <tableColumn id="9" name="Column7" dataDxfId="5"/>
-    <tableColumn id="10" name="Column8" dataDxfId="4"/>
-    <tableColumn id="11" name="Column9" dataDxfId="3"/>
-    <tableColumn id="12" name="Column10" dataDxfId="2"/>
-    <tableColumn id="13" name="Column11" dataDxfId="1"/>
-    <tableColumn id="14" name="Column12" dataDxfId="0"/>
+    <tableColumn id="1" name="Music Genre" dataDxfId="18"/>
+    <tableColumn id="16" name="Column1" dataDxfId="17"/>
+    <tableColumn id="15" name="Using" dataDxfId="16"/>
+    <tableColumn id="2" name="Column13" dataDxfId="15"/>
+    <tableColumn id="3" name="Column2" dataDxfId="14"/>
+    <tableColumn id="4" name="Column3" dataDxfId="13"/>
+    <tableColumn id="5" name="Column4" dataDxfId="12"/>
+    <tableColumn id="6" name="Column5" dataDxfId="11"/>
+    <tableColumn id="8" name="Column52" dataDxfId="10"/>
+    <tableColumn id="7" name="Column6" dataDxfId="9"/>
+    <tableColumn id="9" name="Column7" dataDxfId="8"/>
+    <tableColumn id="10" name="Column8" dataDxfId="7"/>
+    <tableColumn id="11" name="Column9" dataDxfId="6"/>
+    <tableColumn id="12" name="Column10" dataDxfId="5"/>
+    <tableColumn id="13" name="Column11" dataDxfId="4"/>
+    <tableColumn id="14" name="Column12" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:A1048576" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:A1048576"/>
+  <sortState ref="A2:A1048576">
+    <sortCondition ref="A1:A1048576"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Genres" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -762,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1492,12 +1622,257 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="55.42578125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>